<commit_message>
Check-in and some minor updates
Caused the basic version to no longer display the map image
</commit_message>
<xml_diff>
--- a/Simulation_Code_1/Display Simulation/simulationResult.xlsx
+++ b/Simulation_Code_1/Display Simulation/simulationResult.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan.c.larson\Documents\GitHub\SMART_UAV_disaster_algorithm_1\Simulation_Code_1\Display Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27438CEA-25F5-46F5-8CA9-AF66D0908902}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDE13B4-B03A-4DC2-B1CE-A0654FBB3CC8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" activeTab="2" xr2:uid="{BA438FB0-75F3-4A7B-9994-4DA2C0ACA82E}"/>
+    <workbookView xWindow="3816" yWindow="324" windowWidth="9168" windowHeight="8964" activeTab="2" xr2:uid="{BA438FB0-75F3-4A7B-9994-4DA2C0ACA82E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,34 +510,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D2">
-        <v>0.34083333333333332</v>
+        <v>1.3368588490326596</v>
       </c>
       <c r="E2">
-        <v>0.20833333333333337</v>
+        <v>0.41851851851851862</v>
       </c>
       <c r="F2">
-        <v>0.35555555555555551</v>
+        <v>1.4307800191988784</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="J2">
-        <v>58</v>
+        <v>348</v>
       </c>
       <c r="K2">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -577,10 +577,16 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="F2">
+        <v>1.1111111111111112</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -588,16 +594,16 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.1333333333333333</v>
+        <v>0.86041666666666661</v>
       </c>
       <c r="F3">
-        <v>0.1333333333333333</v>
+        <v>0.86041666666666661</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -605,19 +611,19 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.13333333333333336</v>
+        <v>1.5333333333333334</v>
       </c>
       <c r="E4">
-        <v>0.15</v>
+        <v>0.88333333333333341</v>
       </c>
       <c r="F4">
-        <v>0.1166666666666667</v>
+        <v>1.7933333333333334</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -625,16 +631,16 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.5083333333333333</v>
+        <v>1.8250000000000002</v>
       </c>
       <c r="F5">
-        <v>0.5083333333333333</v>
+        <v>1.8250000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -642,10 +648,16 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2.6791666666666667</v>
+      </c>
+      <c r="F6">
+        <v>2.6791666666666667</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -653,10 +665,19 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.81388888888888899</v>
+      </c>
+      <c r="E7">
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="F7">
+        <v>0.93333333333333335</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -664,16 +685,16 @@
         <v>18</v>
       </c>
       <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
       <c r="D8">
-        <v>0.23333333333333336</v>
+        <v>0.4333333333333334</v>
       </c>
       <c r="F8">
-        <v>0.23333333333333336</v>
+        <v>0.4333333333333334</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -681,16 +702,19 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>0.66666666666666674</v>
+        <v>1.6181818181818179</v>
+      </c>
+      <c r="E9">
+        <v>0.1333333333333333</v>
       </c>
       <c r="F9">
-        <v>0.66666666666666674</v>
+        <v>1.7666666666666664</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -698,16 +722,19 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.27500000000000002</v>
+        <v>0.72500000000000009</v>
+      </c>
+      <c r="E10">
+        <v>0.56666666666666687</v>
       </c>
       <c r="F10">
-        <v>0.27500000000000002</v>
+        <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -718,13 +745,13 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0.39166666666666666</v>
+        <v>1.6062500000000002</v>
       </c>
       <c r="F11">
-        <v>0.39166666666666666</v>
+        <v>1.6062500000000002</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -732,16 +759,19 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.6166666666666667</v>
+        <v>0.71333333333333337</v>
+      </c>
+      <c r="E12">
+        <v>0.33333333333333348</v>
       </c>
       <c r="F12">
-        <v>0.6166666666666667</v>
+        <v>0.96666666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -749,16 +779,16 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D13">
-        <v>0.4777777777777778</v>
+        <v>1.392156862745098</v>
       </c>
       <c r="F13">
-        <v>0.4777777777777778</v>
+        <v>1.392156862745098</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -766,19 +796,19 @@
         <v>24</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0.16666666666666669</v>
+        <v>0.82380952380952377</v>
       </c>
       <c r="E14">
-        <v>0.26666666666666672</v>
+        <v>0.20833333333333337</v>
       </c>
       <c r="F14">
-        <v>6.6666666666666652E-2</v>
+        <v>1.0699999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>